<commit_message>
actualizacion del comentario en el excel
</commit_message>
<xml_diff>
--- a/public/archives/PLANTILLA-DE-REGISTRO-PARA-EMPLEADOS.xlsx
+++ b/public/archives/PLANTILLA-DE-REGISTRO-PARA-EMPLEADOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0353DA8-24A8-44B3-A707-63AEC964265F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FE667F-92AF-4062-87DF-D2F81B299475}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDIVIDUAL " sheetId="4" r:id="rId1"/>
@@ -27,73 +27,107 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>sebas arias</author>
+  </authors>
+  <commentList>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{811E827A-961A-45C2-A19C-E17CBEF6EF72}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RED BUCAL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ingrese la cedula del titular al que depende, si no depende, deje el campo vacio</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>CELULAR</t>
-  </si>
-  <si>
-    <t>CORREO</t>
-  </si>
-  <si>
-    <t>F. NACIMIENTO</t>
-  </si>
-  <si>
-    <t>CEDULA</t>
-  </si>
-  <si>
-    <t>PLAN</t>
-  </si>
-  <si>
-    <t>FRECUENCIA</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>IMPUESTO</t>
-  </si>
-  <si>
-    <t>FORMA DE PAGO</t>
-  </si>
-  <si>
     <t>INDIVIDUALES REFERIDOS</t>
   </si>
   <si>
-    <t>CUOTA</t>
-  </si>
-  <si>
-    <t>FECHA</t>
-  </si>
-  <si>
     <t>RED BUCAL S.A.</t>
   </si>
   <si>
     <t xml:space="preserve">MES: </t>
   </si>
   <si>
-    <t>NOMBRE Y APELLIDO</t>
-  </si>
-  <si>
-    <t>DIRECCIÓN</t>
-  </si>
-  <si>
     <t>REPORTE SEMANAL</t>
   </si>
   <si>
-    <t>SE REALIZO LA LIMPIEZA SI/NO</t>
-  </si>
-  <si>
     <t xml:space="preserve">AGENTE: CLINICA </t>
   </si>
   <si>
     <t>Dependiente de quíen?</t>
   </si>
   <si>
-    <t>Provincia</t>
-  </si>
-  <si>
-    <t>corregimiento</t>
+    <t>FECHA*</t>
+  </si>
+  <si>
+    <t>NOMBRE Y APELLIDO*</t>
+  </si>
+  <si>
+    <t>CEDULA*</t>
+  </si>
+  <si>
+    <t>F. NACIMIENTO*</t>
+  </si>
+  <si>
+    <t>Provincia*</t>
+  </si>
+  <si>
+    <t>corregimiento*</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN*</t>
+  </si>
+  <si>
+    <t>CELULAR*</t>
+  </si>
+  <si>
+    <t>CORREO*</t>
+  </si>
+  <si>
+    <t>PLAN*</t>
+  </si>
+  <si>
+    <t>CUOTA*</t>
+  </si>
+  <si>
+    <t>IMPUESTO*</t>
+  </si>
+  <si>
+    <t>TOTAL*</t>
+  </si>
+  <si>
+    <t>FRECUENCIA*</t>
+  </si>
+  <si>
+    <t>FORMA DE PAGO*</t>
+  </si>
+  <si>
+    <t>SE REALIZO LA LIMPIEZA* SI/NO</t>
   </si>
 </sst>
 </file>
@@ -103,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;B/.&quot;* #,##0.00_-;\-&quot;B/.&quot;* #,##0.00_-;_-&quot;B/.&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +180,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -611,11 +658,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A13" sqref="A13:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,8 +676,9 @@
     <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" customWidth="1"/>
     <col min="16" max="17" width="24" customWidth="1"/>
     <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -732,7 +780,7 @@
     </row>
     <row r="6" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -755,7 +803,7 @@
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -776,7 +824,7 @@
     </row>
     <row r="8" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -797,7 +845,7 @@
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -818,7 +866,7 @@
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -858,55 +906,55 @@
     </row>
     <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="H12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="K12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="P12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="Q12" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1398,5 +1446,6 @@
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-imagen de pago de index cambiada a blanco - excel de registro actualizado el comentario - mapa arreglado
</commit_message>
<xml_diff>
--- a/public/archives/PLANTILLA-DE-REGISTRO-PARA-EMPLEADOS.xlsx
+++ b/public/archives/PLANTILLA-DE-REGISTRO-PARA-EMPLEADOS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FE667F-92AF-4062-87DF-D2F81B299475}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E90B6E-4B2E-4C4D-9C43-84F47D05D4FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDIVIDUAL " sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'INDIVIDUAL '!$A$1:$P$37</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +53,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Ingrese la cedula del titular al que depende, si no depende, deje el campo vacio</t>
+Si el individuo es dependiente de otro usuario, diligencie el número de documento del usuario principal en este campo. De lo contrario deje este espacio vacío.</t>
         </r>
       </text>
     </comment>
@@ -79,9 +79,6 @@
     <t xml:space="preserve">AGENTE: CLINICA </t>
   </si>
   <si>
-    <t>Dependiente de quíen?</t>
-  </si>
-  <si>
     <t>FECHA*</t>
   </si>
   <si>
@@ -94,12 +91,6 @@
     <t>F. NACIMIENTO*</t>
   </si>
   <si>
-    <t>Provincia*</t>
-  </si>
-  <si>
-    <t>corregimiento*</t>
-  </si>
-  <si>
     <t>DIRECCIÓN*</t>
   </si>
   <si>
@@ -128,6 +119,36 @@
   </si>
   <si>
     <t>SE REALIZO LA LIMPIEZA* SI/NO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dependiente de quíen?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(Si el individuo es dependiente de otro usuario, diligencie el número de documento del usuario principal en este campo. De lo contrario deje este espacio vacío.)</t>
+    </r>
+  </si>
+  <si>
+    <t>PROVINCIA*</t>
+  </si>
+  <si>
+    <t>CORREGIMIENTO*</t>
   </si>
 </sst>
 </file>
@@ -137,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;B/.&quot;* #,##0.00_-;\-&quot;B/.&quot;* #,##0.00_-;_-&quot;B/.&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +214,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -256,7 +285,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -270,9 +299,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -290,6 +316,12 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -661,303 +693,303 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:Q16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13:L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="31.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="31.109375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="31.109375" style="10" customWidth="1"/>
-    <col min="8" max="9" width="31.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="31.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="31.140625" style="9" customWidth="1"/>
+    <col min="8" max="9" width="31.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
     <col min="16" max="17" width="24" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-    </row>
-    <row r="6" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+    </row>
+    <row r="6" spans="1:19" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:19" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-    </row>
-    <row r="8" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+    </row>
+    <row r="8" spans="1:19" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-    </row>
-    <row r="9" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+    </row>
+    <row r="9" spans="1:19" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-    </row>
-    <row r="10" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-    </row>
-    <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="I12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="J12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="K12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="L12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="M12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="N12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="O12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="P12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="Q12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="O12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -967,7 +999,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="11"/>
+      <c r="J13" s="10"/>
       <c r="K13" s="5"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -976,7 +1008,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -986,7 +1018,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="11"/>
+      <c r="J14" s="10"/>
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
@@ -995,7 +1027,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1005,7 +1037,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="11"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="5"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
@@ -1014,7 +1046,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1024,7 +1056,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="11"/>
+      <c r="J16" s="10"/>
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
@@ -1033,7 +1065,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1043,7 +1075,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="11"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -1052,7 +1084,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1071,7 +1103,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1090,7 +1122,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1109,7 +1141,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1128,7 +1160,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1147,7 +1179,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1166,7 +1198,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1185,7 +1217,7 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1204,7 +1236,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1223,7 +1255,7 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1242,7 +1274,7 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1261,7 +1293,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1280,7 +1312,7 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1299,7 +1331,7 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1318,7 +1350,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1337,7 +1369,7 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1356,7 +1388,7 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1375,7 +1407,7 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1394,7 +1426,7 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1413,7 +1445,7 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>

</xml_diff>